<commit_message>
week 7 and 8
</commit_message>
<xml_diff>
--- a/data/w3_exercise.xlsx
+++ b/data/w3_exercise.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorfrench/Dropbox/Old_Mac/School_Stuff/CUNY/teaching/dss_2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0C6AC85-9A9B-3248-B221-81EAA7BD4597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B604009-57AB-D646-8BC2-06F319051660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{F800DD34-4575-884B-9E70-07AD2FD20636}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{F800DD34-4575-884B-9E70-07AD2FD20636}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Pokemon</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Woobat</t>
+  </si>
+  <si>
+    <t>Caterpie HP</t>
+  </si>
+  <si>
+    <t>CP minimum</t>
   </si>
 </sst>
 </file>
@@ -446,19 +452,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2E52F3-042E-2A46-A96A-CD5466C10367}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +478,23 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -479,8 +504,11 @@
       <c r="C2">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -491,7 +519,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -502,7 +530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -513,7 +541,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -524,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -535,7 +563,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -546,7 +574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -557,7 +585,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -568,7 +596,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>

</xml_diff>